<commit_message>
Update DU for 2 October
</commit_message>
<xml_diff>
--- a/testing/TestCases.xlsx
+++ b/testing/TestCases.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Iteration1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
-    <sheet name="Iteration2" sheetId="4" r:id="rId3"/>
+    <sheet name="Iteration1-Manual-Login" sheetId="2" r:id="rId1"/>
+    <sheet name="Iteration2-Manual-bootstrap-bid" sheetId="4" r:id="rId2"/>
+    <sheet name="Iteration1-JSON-Login" sheetId="5" r:id="rId3"/>
+    <sheet name="Iteration2-JSON-authenticate" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="205">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -980,6 +981,9 @@
 course: IS108
 section:S1
 bid amount:abc123</t>
+  </si>
+  <si>
+    <t>Bidding (add)</t>
   </si>
 </sst>
 </file>
@@ -1140,11 +1144,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -1169,13 +1173,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>977900</xdr:colOff>
+      <xdr:colOff>917742</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>673101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>244642</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>774700</xdr:rowOff>
     </xdr:to>
@@ -1193,8 +1197,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11061700" y="2222501"/>
-          <a:ext cx="3708400" cy="901699"/>
+          <a:off x="10974137" y="2568075"/>
+          <a:ext cx="3718426" cy="903704"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1663,6 +1667,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>2686539</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>591620</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1404148</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20161250" y="36964327"/>
+          <a:ext cx="10971428" cy="1428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1867,7 +1909,7 @@
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1931,8 +1973,8 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
     </row>
-    <row r="2" spans="1:28" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:28" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2233,22 +2275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D32" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2312,18 +2342,18 @@
       <c r="AA1" s="14"/>
       <c r="AB1" s="14"/>
     </row>
-    <row r="2" spans="1:28" s="18" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:28" s="19" customFormat="1" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:28" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:28" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>67</v>
@@ -2348,8 +2378,8 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>45</v>
+      <c r="B5" t="s">
+        <v>204</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>48</v>
@@ -2375,7 +2405,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>47</v>
@@ -2427,7 +2457,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>63</v>
@@ -2453,7 +2483,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>65</v>
@@ -2479,7 +2509,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>64</v>
@@ -2493,7 +2523,7 @@
       <c r="F10" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="17" t="s">
         <v>190</v>
       </c>
       <c r="H10" t="s">
@@ -2505,7 +2535,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>49</v>
@@ -2531,7 +2561,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>71</v>
@@ -2557,9 +2587,9 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -2583,9 +2613,9 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="7" t="s">
@@ -2609,7 +2639,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>9</v>
@@ -2635,9 +2665,9 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -2661,9 +2691,9 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2819,7 +2849,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>64</v>
@@ -2840,12 +2870,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+    <row r="27" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="17" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:8" s="18" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:8" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
@@ -3089,4 +3119,30 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>